<commit_message>
Aplicacion - ABC Consumos. TODO: Mensaje de duplicado  y Usuario_Mod
</commit_message>
<xml_diff>
--- a/My Project/Archivos_Carga/Carga_Consumos.xlsx
+++ b/My Project/Archivos_Carga/Carga_Consumos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RESPALDO\ESCUELA\MAD - 001\PIA - Nuevo\PIA MAD\Aplicacion\PIA MAD - ScdChnc\My Project\Archivos_Carga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318D653D-F72E-485D-AC90-4941A5A01B37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7855C7E-16AF-47E6-AE10-1F37E0036D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4CBCFDA4-C8AA-47A7-8A50-858439D32C05}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B26766-6072-44FE-8B21-C45C0592F3CC}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,38 +430,10 @@
         <v>2021</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2021</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2021</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>